<commit_message>
Atulaizando Relatório, Adição de um novo membro
</commit_message>
<xml_diff>
--- a/Cronograma/CRONOGRAMA PIM.xlsx
+++ b/Cronograma/CRONOGRAMA PIM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cedc36dc4fb55eb/Unip/Pim/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GIT-HUB\Pim-Enfermagem\Cronograma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="5_{34EA1EAE-27E7-4CEE-B299-AC4608A345C8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A0252AD7-F707-4B7D-8925-F7B2CE6002FD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9AB880-E255-44FD-86A1-57C583EAE2EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
   <si>
     <t xml:space="preserve">Sinalizador de Porcentagem Acima/Abaixo: </t>
   </si>
@@ -224,6 +224,18 @@
   </si>
   <si>
     <t>Adriel</t>
+  </si>
+  <si>
+    <t>(15)99813-8622</t>
+  </si>
+  <si>
+    <t>Kaique</t>
+  </si>
+  <si>
+    <t>(15)99666-1049</t>
+  </si>
+  <si>
+    <t>paulorossifrias@hotmail.com</t>
   </si>
 </sst>
 </file>
@@ -649,20 +661,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="2" applyProtection="1">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="3" xfId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6">
@@ -671,7 +680,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -692,9 +701,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="16" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -707,49 +713,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="5" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="8" applyFont="1">
+      <alignment horizontal="right" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="4" applyFont="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="16" fillId="2" borderId="0" xfId="15" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="3" fontId="16" fillId="2" borderId="0" xfId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="5" xfId="13" applyFont="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="12" applyFont="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="2" borderId="0" xfId="14" applyFont="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="5" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="12" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="16" fillId="2" borderId="0" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
@@ -777,6 +780,58 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -791,40 +846,154 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Century Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <name val="Century Gothic"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1144,224 +1313,6 @@
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
         <top/>
@@ -1369,6 +1320,42 @@
           <color theme="9"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <name val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1902,13 +1889,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>1732540</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>119784</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>665740</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>23091</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2059,50 +2046,50 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Controlador_de_projeto" displayName="Controlador_de_projeto" ref="B4:O13" totalsRowShown="0" headerRowDxfId="2" dataDxfId="3" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Controlador_de_projeto" displayName="Controlador_de_projeto" ref="B4:O13" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
   <autoFilter ref="B4:O13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState ref="B5:O13">
     <sortCondition sortBy="icon" ref="C5:C13"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Atividades" dataDxfId="17" dataCellStyle="Texto"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prioridade" dataDxfId="16" dataCellStyle="Texto"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Atribuída a" dataDxfId="15" dataCellStyle="Texto"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Estimado_x000a_Início" dataDxfId="14" dataCellStyle="Data"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Estimado _x000a_Término" dataDxfId="13" dataCellStyle="Data"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Trabalho Estimado (em horas)" dataDxfId="12" dataCellStyle="Números"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Duração Estimada (em dias)" dataDxfId="11" dataCellStyle="Duração estimada">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Atividades" dataDxfId="28" dataCellStyle="Texto"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prioridade" dataDxfId="27" dataCellStyle="Texto"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Atribuída a" dataDxfId="26" dataCellStyle="Texto"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Estimado_x000a_Início" dataDxfId="25" dataCellStyle="Data"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Estimado _x000a_Término" dataDxfId="24" dataCellStyle="Data"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Trabalho Estimado (em horas)" dataDxfId="23" dataCellStyle="Números"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Duração Estimada (em dias)" dataDxfId="22" dataCellStyle="Duração estimada">
       <calculatedColumnFormula>IF(COUNTA(Cronograma!$E5,Cronograma!$F5)&lt;&gt;2,"",DAYS360(Cronograma!$E5,Cronograma!$F5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Real _x000a_Início" dataDxfId="10" dataCellStyle="Início Real"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Real_x000a_Término" dataDxfId="9" dataCellStyle="Data"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ícone de sinalizador para o trabalho real de acima/abaixo (em horas)" dataDxfId="8" dataCellStyle="Sinalizador">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Real _x000a_Início" dataDxfId="21" dataCellStyle="Início Real"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Real_x000a_Término" dataDxfId="20" dataCellStyle="Data"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ícone de sinalizador para o trabalho real de acima/abaixo (em horas)" dataDxfId="19" dataCellStyle="Sinalizador">
       <calculatedColumnFormula>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Trabalho Real (em horas)" dataDxfId="7" dataCellStyle="Números"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Ícone de sinalizador para duração real acima/abaixo (em dias)" dataDxfId="6" dataCellStyle="Sinalizador">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Trabalho Real (em horas)" dataDxfId="18" dataCellStyle="Números"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Ícone de sinalizador para duração real acima/abaixo (em dias)" dataDxfId="17" dataCellStyle="Sinalizador">
       <calculatedColumnFormula>IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Duração Real (em dias)" dataDxfId="5" dataCellStyle="Coluna cinza">
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Duração Real (em dias)" dataDxfId="16" dataCellStyle="Coluna cinza">
       <calculatedColumnFormula>IF(COUNTA(Cronograma!$I5,Cronograma!$J5)&lt;&gt;2,"",DAYS360(Cronograma!$I5,Cronograma!$J5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Anotações" dataDxfId="4" dataCellStyle="Texto"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Anotações" dataDxfId="15" dataCellStyle="Texto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5EF5E39F-083C-4CBF-9C73-059A3E5DC12C}" name="TabelaInformações" displayName="TabelaInformações" ref="B2:E9" totalsRowCount="1" headerRowDxfId="19" totalsRowDxfId="18" headerRowBorderDxfId="29" tableBorderDxfId="30" totalsRowBorderDxfId="28">
-  <autoFilter ref="B2:E8" xr:uid="{80914F49-B214-4A9D-9AA6-C62850A3AF1D}"/>
-  <sortState ref="B3:E7">
-    <sortCondition ref="B2:B8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5EF5E39F-083C-4CBF-9C73-059A3E5DC12C}" name="TabelaInformações" displayName="TabelaInformações" ref="B2:E10" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="11" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="10">
+  <autoFilter ref="B2:E9" xr:uid="{80914F49-B214-4A9D-9AA6-C62850A3AF1D}"/>
+  <sortState ref="B3:E8">
+    <sortCondition ref="B2:B9"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{015C0AFA-387D-445F-B28F-76D6562120F5}" name="Nome" totalsRowFunction="count" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{99352CCE-884C-490C-9AA3-B8279BA0B565}" name="E-mail" totalsRowFunction="count" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{942D1AB5-65C0-4A7C-8B7B-DD05F2AB2033}" name="Celular" totalsRowFunction="count" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{9BE67810-E51A-4696-888C-21CED24CD269}" name="Git-Hub" totalsRowFunction="count" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="1" xr3:uid="{015C0AFA-387D-445F-B28F-76D6562120F5}" name="Nome" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{99352CCE-884C-490C-9AA3-B8279BA0B565}" name="E-mail" totalsRowFunction="count" dataDxfId="8" totalsRowDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{942D1AB5-65C0-4A7C-8B7B-DD05F2AB2033}" name="Celular" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{9BE67810-E51A-4696-888C-21CED24CD269}" name="Git-Hub" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2356,7 +2343,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -2381,549 +2368,544 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="38.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="2" customWidth="1"/>
-    <col min="6" max="6" width="14.875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="2.875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="12.875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="2.875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.25" style="1" customWidth="1"/>
-    <col min="15" max="15" width="25.625" style="1" customWidth="1"/>
-    <col min="16" max="16" width="2.625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="38.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="5" width="15" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.125" customWidth="1"/>
+    <col min="9" max="9" width="15.375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="15.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="2.875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.875" customWidth="1"/>
+    <col min="13" max="13" width="2.875" customWidth="1"/>
+    <col min="14" max="14" width="13.25" customWidth="1"/>
+    <col min="15" max="15" width="25.625" customWidth="1"/>
+    <col min="16" max="16" width="2.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="C1"/>
     </row>
     <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="G3"/>
-      <c r="H3"/>
-    </row>
+    <row r="3" spans="1:15" ht="16.5" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="23" t="s">
+      <c r="H4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="25" t="s">
+      <c r="K4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="22" t="s">
+      <c r="L4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="25" t="s">
+      <c r="M4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="20" t="s">
+      <c r="O4" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="24">
         <f ca="1">TODAY()+6</f>
-        <v>43534</v>
-      </c>
-      <c r="F5" s="27">
+        <v>43545</v>
+      </c>
+      <c r="F5" s="24">
         <f ca="1">TODAY()+30</f>
-        <v>43558</v>
-      </c>
-      <c r="G5" s="28">
+        <v>43569</v>
+      </c>
+      <c r="G5" s="25">
         <v>210</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E5,Cronograma!$F5)&lt;&gt;2,"",DAYS360(Cronograma!$E5,Cronograma!$F5,FALSE))</f>
         <v>23</v>
       </c>
-      <c r="I5" s="30">
+      <c r="I5" s="27">
         <f ca="1">TODAY()-65</f>
-        <v>43463</v>
-      </c>
-      <c r="J5" s="27">
+        <v>43474</v>
+      </c>
+      <c r="J5" s="24">
         <f ca="1">TODAY()</f>
-        <v>43528</v>
-      </c>
-      <c r="K5" s="31">
+        <v>43539</v>
+      </c>
+      <c r="K5" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>1</v>
       </c>
-      <c r="L5" s="28">
+      <c r="L5" s="25">
         <v>300</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>1</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I5,Cronograma!$J5)&lt;&gt;2,"",DAYS360(Cronograma!$I5,Cronograma!$J5,FALSE))</f>
-        <v>65</v>
-      </c>
-      <c r="O5" s="26"/>
+        <v>66</v>
+      </c>
+      <c r="O5" s="23"/>
     </row>
     <row r="6" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="24">
         <f ca="1">TODAY()-35</f>
-        <v>43493</v>
-      </c>
-      <c r="F6" s="27">
+        <v>43504</v>
+      </c>
+      <c r="F6" s="24">
         <f ca="1">TODAY()+20</f>
-        <v>43548</v>
-      </c>
-      <c r="G6" s="28">
+        <v>43559</v>
+      </c>
+      <c r="G6" s="25">
         <v>400</v>
       </c>
-      <c r="H6" s="29">
+      <c r="H6" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E6,Cronograma!$F6)&lt;&gt;2,"",DAYS360(Cronograma!$E6,Cronograma!$F6,FALSE))</f>
         <v>56</v>
       </c>
-      <c r="I6" s="30">
+      <c r="I6" s="27">
         <f ca="1">TODAY()-41</f>
-        <v>43487</v>
-      </c>
-      <c r="J6" s="27">
+        <v>43498</v>
+      </c>
+      <c r="J6" s="24">
         <f ca="1">TODAY()-7</f>
-        <v>43521</v>
-      </c>
-      <c r="K6" s="31">
+        <v>43532</v>
+      </c>
+      <c r="K6" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L6" s="28">
+      <c r="L6" s="25">
         <v>390</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>1</v>
       </c>
-      <c r="N6" s="32">
+      <c r="N6" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I6,Cronograma!$J6)&lt;&gt;2,"",DAYS360(Cronograma!$I6,Cronograma!$J6,FALSE))</f>
+        <v>36</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="27">
+      <c r="E7" s="24">
         <f ca="1">TODAY()+8</f>
-        <v>43536</v>
-      </c>
-      <c r="F7" s="27">
+        <v>43547</v>
+      </c>
+      <c r="F7" s="24">
         <f ca="1">TODAY()+30</f>
-        <v>43558</v>
-      </c>
-      <c r="G7" s="28">
+        <v>43569</v>
+      </c>
+      <c r="G7" s="25">
         <v>500</v>
       </c>
-      <c r="H7" s="29">
+      <c r="H7" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E7,Cronograma!$F7)&lt;&gt;2,"",DAYS360(Cronograma!$E7,Cronograma!$F7,FALSE))</f>
         <v>21</v>
       </c>
-      <c r="I7" s="30">
+      <c r="I7" s="27">
         <f ca="1">TODAY()-100</f>
-        <v>43428</v>
-      </c>
-      <c r="J7" s="27">
+        <v>43439</v>
+      </c>
+      <c r="J7" s="24">
         <f ca="1">TODAY()-27</f>
-        <v>43501</v>
-      </c>
-      <c r="K7" s="31">
+        <v>43512</v>
+      </c>
+      <c r="K7" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L7" s="28">
+      <c r="L7" s="25">
         <v>500</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>1</v>
       </c>
-      <c r="N7" s="32">
+      <c r="N7" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I7,Cronograma!$J7)&lt;&gt;2,"",DAYS360(Cronograma!$I7,Cronograma!$J7,FALSE))</f>
         <v>71</v>
       </c>
-      <c r="O7" s="26"/>
+      <c r="O7" s="23"/>
     </row>
     <row r="8" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="24">
         <f ca="1">TODAY()+9</f>
-        <v>43537</v>
-      </c>
-      <c r="F8" s="27">
+        <v>43548</v>
+      </c>
+      <c r="F8" s="24">
         <f ca="1">TODAY()+30</f>
-        <v>43558</v>
-      </c>
-      <c r="G8" s="28">
+        <v>43569</v>
+      </c>
+      <c r="G8" s="25">
         <v>250</v>
       </c>
-      <c r="H8" s="29">
+      <c r="H8" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E8,Cronograma!$F8)&lt;&gt;2,"",DAYS360(Cronograma!$E8,Cronograma!$F8,FALSE))</f>
         <v>20</v>
       </c>
-      <c r="I8" s="30">
+      <c r="I8" s="27">
         <f ca="1">TODAY()-90</f>
-        <v>43438</v>
-      </c>
-      <c r="J8" s="27">
+        <v>43449</v>
+      </c>
+      <c r="J8" s="24">
         <f ca="1">TODAY()-71</f>
-        <v>43457</v>
-      </c>
-      <c r="K8" s="31">
+        <v>43468</v>
+      </c>
+      <c r="K8" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="25">
         <v>276</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="N8" s="32">
+      <c r="N8" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I8,Cronograma!$J8)&lt;&gt;2,"",DAYS360(Cronograma!$I8,Cronograma!$J8,FALSE))</f>
-        <v>19</v>
-      </c>
-      <c r="O8" s="26"/>
+        <v>18</v>
+      </c>
+      <c r="O8" s="23"/>
     </row>
     <row r="9" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="24">
         <f ca="1">TODAY()+10</f>
-        <v>43538</v>
-      </c>
-      <c r="F9" s="27">
+        <v>43549</v>
+      </c>
+      <c r="F9" s="24">
         <f ca="1">TODAY()+30</f>
-        <v>43558</v>
-      </c>
-      <c r="G9" s="28">
+        <v>43569</v>
+      </c>
+      <c r="G9" s="25">
         <v>300</v>
       </c>
-      <c r="H9" s="29">
+      <c r="H9" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E9,Cronograma!$F9)&lt;&gt;2,"",DAYS360(Cronograma!$E9,Cronograma!$F9,FALSE))</f>
         <v>19</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="27">
         <f ca="1">TODAY()-90</f>
-        <v>43438</v>
-      </c>
-      <c r="J9" s="27">
+        <v>43449</v>
+      </c>
+      <c r="J9" s="24">
         <f ca="1">TODAY()-44</f>
-        <v>43484</v>
-      </c>
-      <c r="K9" s="31">
+        <v>43495</v>
+      </c>
+      <c r="K9" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L9" s="28">
+      <c r="L9" s="25">
         <v>310</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>1</v>
       </c>
-      <c r="N9" s="32">
+      <c r="N9" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I9,Cronograma!$J9)&lt;&gt;2,"",DAYS360(Cronograma!$I9,Cronograma!$J9,FALSE))</f>
         <v>45</v>
       </c>
-      <c r="O9" s="26"/>
+      <c r="O9" s="23"/>
     </row>
     <row r="10" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="24">
         <f ca="1">TODAY()+11</f>
-        <v>43539</v>
-      </c>
-      <c r="F10" s="27">
+        <v>43550</v>
+      </c>
+      <c r="F10" s="24">
         <f ca="1">TODAY()+30</f>
-        <v>43558</v>
-      </c>
-      <c r="G10" s="28">
+        <v>43569</v>
+      </c>
+      <c r="G10" s="25">
         <v>500</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E10,Cronograma!$F10)&lt;&gt;2,"",DAYS360(Cronograma!$E10,Cronograma!$F10,FALSE))</f>
         <v>18</v>
       </c>
-      <c r="I10" s="30">
+      <c r="I10" s="27">
         <f ca="1">TODAY()-60</f>
-        <v>43468</v>
-      </c>
-      <c r="J10" s="27">
+        <v>43479</v>
+      </c>
+      <c r="J10" s="24">
         <f ca="1">TODAY()-45</f>
-        <v>43483</v>
-      </c>
-      <c r="K10" s="31">
+        <v>43494</v>
+      </c>
+      <c r="K10" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L10" s="28">
+      <c r="L10" s="25">
         <v>510</v>
       </c>
-      <c r="M10" s="31">
+      <c r="M10" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="N10" s="32">
+      <c r="N10" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I10,Cronograma!$J10)&lt;&gt;2,"",DAYS360(Cronograma!$I10,Cronograma!$J10,FALSE))</f>
         <v>15</v>
       </c>
-      <c r="O10" s="26"/>
+      <c r="O10" s="23"/>
     </row>
     <row r="11" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="24">
         <f ca="1">TODAY()-44</f>
-        <v>43484</v>
-      </c>
-      <c r="F11" s="27">
+        <v>43495</v>
+      </c>
+      <c r="F11" s="24">
         <f ca="1">TODAY()+30</f>
-        <v>43558</v>
-      </c>
-      <c r="G11" s="28">
+        <v>43569</v>
+      </c>
+      <c r="G11" s="25">
         <v>750</v>
       </c>
-      <c r="H11" s="29">
+      <c r="H11" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E11,Cronograma!$F11)&lt;&gt;2,"",DAYS360(Cronograma!$E11,Cronograma!$F11,FALSE))</f>
         <v>74</v>
       </c>
-      <c r="I11" s="30">
+      <c r="I11" s="27">
         <f ca="1">TODAY()-44</f>
-        <v>43484</v>
-      </c>
-      <c r="J11" s="27">
+        <v>43495</v>
+      </c>
+      <c r="J11" s="24">
         <f ca="1">TODAY()-15</f>
-        <v>43513</v>
-      </c>
-      <c r="K11" s="31">
+        <v>43524</v>
+      </c>
+      <c r="K11" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L11" s="28">
+      <c r="L11" s="25">
         <v>790</v>
       </c>
-      <c r="M11" s="31">
+      <c r="M11" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>1</v>
       </c>
-      <c r="N11" s="32">
+      <c r="N11" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I11,Cronograma!$J11)&lt;&gt;2,"",DAYS360(Cronograma!$I11,Cronograma!$J11,FALSE))</f>
         <v>28</v>
       </c>
-      <c r="O11" s="26"/>
+      <c r="O11" s="23"/>
     </row>
     <row r="12" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="24">
         <f ca="1">TODAY()+20</f>
-        <v>43548</v>
-      </c>
-      <c r="F12" s="27">
+        <v>43559</v>
+      </c>
+      <c r="F12" s="24">
         <f ca="1">TODAY()+60</f>
-        <v>43588</v>
-      </c>
-      <c r="G12" s="28">
+        <v>43599</v>
+      </c>
+      <c r="G12" s="25">
         <v>450</v>
       </c>
-      <c r="H12" s="29">
+      <c r="H12" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E12,Cronograma!$F12)&lt;&gt;2,"",DAYS360(Cronograma!$E12,Cronograma!$F12,FALSE))</f>
-        <v>39</v>
-      </c>
-      <c r="I12" s="30">
+        <v>40</v>
+      </c>
+      <c r="I12" s="27">
         <f ca="1">TODAY()-45</f>
-        <v>43483</v>
-      </c>
-      <c r="J12" s="27">
+        <v>43494</v>
+      </c>
+      <c r="J12" s="24">
         <f ca="1">TODAY()-5</f>
-        <v>43523</v>
-      </c>
-      <c r="K12" s="31">
+        <v>43534</v>
+      </c>
+      <c r="K12" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12" s="25">
         <v>430</v>
       </c>
-      <c r="M12" s="31">
+      <c r="M12" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="N12" s="32">
+      <c r="N12" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I12,Cronograma!$J12)&lt;&gt;2,"",DAYS360(Cronograma!$I12,Cronograma!$J12,FALSE))</f>
+        <v>41</v>
+      </c>
+      <c r="O12" s="23"/>
+    </row>
+    <row r="13" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="O12" s="26"/>
-    </row>
-    <row r="13" spans="1:15" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="27">
+      <c r="E13" s="24">
         <f ca="1">TODAY()-160</f>
-        <v>43368</v>
-      </c>
-      <c r="F13" s="27">
+        <v>43379</v>
+      </c>
+      <c r="F13" s="24">
         <f ca="1">TODAY()+91</f>
-        <v>43619</v>
-      </c>
-      <c r="G13" s="28">
+        <v>43630</v>
+      </c>
+      <c r="G13" s="25">
         <v>250</v>
       </c>
-      <c r="H13" s="29">
+      <c r="H13" s="26">
         <f ca="1">IF(COUNTA(Cronograma!$E13,Cronograma!$F13)&lt;&gt;2,"",DAYS360(Cronograma!$E13,Cronograma!$F13,FALSE))</f>
         <v>248</v>
       </c>
-      <c r="I13" s="30">
+      <c r="I13" s="27">
         <v>42434</v>
       </c>
-      <c r="J13" s="27">
+      <c r="J13" s="24">
         <v>42495</v>
       </c>
-      <c r="K13" s="31">
+      <c r="K13" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
         <v>0</v>
       </c>
-      <c r="L13" s="28">
+      <c r="L13" s="25">
         <v>200</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
         <v>1</v>
       </c>
-      <c r="N13" s="32">
+      <c r="N13" s="29">
         <f>IF(COUNTA(Cronograma!$I13,Cronograma!$J13)&lt;&gt;2,"",DAYS360(Cronograma!$I13,Cronograma!$J13,FALSE))</f>
         <v>60</v>
       </c>
-      <c r="O13" s="26"/>
+      <c r="O13" s="23"/>
     </row>
     <row r="17" spans="3:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="7"/>
+      <c r="C17" s="6"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="L5:L13">
-    <cfRule type="expression" dxfId="1" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>(ABS((L5-G5))/G5)&gt;FlagPercent</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:N13">
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>(ABS((N5-H5))/H5)&gt;FlagPercent</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3010,9 +2992,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DD9322-CF5B-4EA7-B626-99B03376E7BD}">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3023,103 +3007,121 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="13"/>
+    </row>
+    <row r="7" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+    <row r="8" spans="2:5" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="11"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B9" s="16">
+    <row r="9" spans="2:5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="14">
         <f>SUBTOTAL(103,TabelaInformações[Nome])</f>
-        <v>5</v>
-      </c>
-      <c r="C9" s="17">
+        <v>6</v>
+      </c>
+      <c r="C10" s="15">
         <f>SUBTOTAL(103,TabelaInformações[E-mail])</f>
-        <v>2</v>
-      </c>
-      <c r="D9" s="17">
+        <v>3</v>
+      </c>
+      <c r="D10" s="15">
         <f>SUBTOTAL(103,TabelaInformações[Celular])</f>
-        <v>5</v>
-      </c>
-      <c r="E9" s="18">
+        <v>6</v>
+      </c>
+      <c r="E10" s="16">
         <f>SUBTOTAL(103,TabelaInformações[Git-Hub])</f>
         <v>5</v>
       </c>
@@ -3129,11 +3131,17 @@
     <hyperlink ref="C3" r:id="rId1" xr:uid="{10E1A243-1F9D-4653-9CB3-246FAAEFFFC9}"/>
     <hyperlink ref="C4" r:id="rId2" xr:uid="{5E2A8B4C-3175-420D-9022-5F5D373DE07E}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{A208A63A-DA4E-48D4-ACA4-51055CB62F93}"/>
+    <hyperlink ref="E3" r:id="rId4" xr:uid="{6E583752-D9C6-4B44-A385-99315902FAAA}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{8169B9CF-DAC7-4769-B26B-3A29711DE9E2}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{9ACC969C-4C4F-4DD2-9241-A3B590E23052}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{4AFB3E2B-1BA3-4670-9BC2-50B1056D2DED}"/>
+    <hyperlink ref="E8" r:id="rId8" xr:uid="{613390DA-BE61-41F9-8193-624ACF60D985}"/>
+    <hyperlink ref="C5" r:id="rId9" xr:uid="{B644CA9E-9055-46BC-9292-573A237280C1}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>
@@ -3159,98 +3167,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="34"/>
+      <c r="C1" s="31"/>
     </row>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="2:3" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6" t="s">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="2:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Atualização no software 03.06
</commit_message>
<xml_diff>
--- a/Cronograma/CRONOGRAMA PIM.xlsx
+++ b/Cronograma/CRONOGRAMA PIM.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GIT-HUB\Pim-Enfermagem\Cronograma\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9AB880-E255-44FD-86A1-57C583EAE2EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19800" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="4" r:id="rId1"/>
-    <sheet name="Cronograma" sheetId="1" r:id="rId2"/>
-    <sheet name="Informações" sheetId="5" r:id="rId3"/>
-    <sheet name="Configuração" sheetId="2" r:id="rId4"/>
+    <sheet name="Gráf2" sheetId="7" r:id="rId2"/>
+    <sheet name="Gráf1" sheetId="6" r:id="rId3"/>
+    <sheet name="Cronograma" sheetId="1" r:id="rId4"/>
+    <sheet name="Informações" sheetId="5" r:id="rId5"/>
+    <sheet name="Configuração" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="CategoryList">Configuração!$B$5:$B$17</definedName>
@@ -24,9 +20,9 @@
     <definedName name="ColumnTitle2">CategoryAndEmployeeTable[[#Headers],[Nome da Categoria]]</definedName>
     <definedName name="EmployeeList">Configuração!$C$5:$C$14</definedName>
     <definedName name="FlagPercent">Cronograma!$C$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">Cronograma!$4:$4</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">Cronograma!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -241,7 +237,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;Over/Under flag&quot;;&quot;&quot;;&quot;&quot;"/>
   </numFmts>
@@ -661,7 +657,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -755,23 +751,26 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="9" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
-    <cellStyle name="Coluna cinza" xfId="14" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Data" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Duração estimada" xfId="15" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Coluna cinza" xfId="14"/>
+    <cellStyle name="Data" xfId="8"/>
+    <cellStyle name="Duração estimada" xfId="15"/>
     <cellStyle name="Entrada" xfId="2" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Hiperlink" xfId="16" builtinId="8"/>
-    <cellStyle name="Início Real" xfId="13" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Início Real" xfId="13"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Nota" xfId="7" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Números" xfId="4" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Números" xfId="4"/>
     <cellStyle name="Saída" xfId="3" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Sinalizador" xfId="12" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Texto" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Sinalizador" xfId="12"/>
+    <cellStyle name="Texto" xfId="5"/>
     <cellStyle name="Título" xfId="9" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Título 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="6" builtinId="17" customBuiltin="1"/>
@@ -830,20 +829,6 @@
         </top>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
     </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
@@ -1009,7 +994,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1029,7 +1013,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -1055,7 +1038,6 @@
         <sz val="12"/>
         <color theme="0"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Over/Under flag&quot;;&quot;&quot;;&quot;&quot;"/>
@@ -1083,7 +1065,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -1103,7 +1084,6 @@
         <sz val="12"/>
         <color theme="0"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="164" formatCode="&quot;Over/Under flag&quot;;&quot;&quot;;&quot;&quot;"/>
@@ -1131,7 +1111,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89992980742820516"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1151,7 +1130,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89992980742820516"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1179,7 +1157,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -1205,7 +1182,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -1225,7 +1201,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89992980742820516"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1245,7 +1220,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89992980742820516"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -1265,7 +1239,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1285,7 +1258,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1305,7 +1277,6 @@
         <sz val="12"/>
         <color theme="2" tint="-0.89989928891872917"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1332,7 +1303,6 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
     </dxf>
@@ -1347,7 +1317,6 @@
         <vertAlign val="baseline"/>
         <sz val="14"/>
         <name val="Century Gothic"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -1356,6 +1325,20 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1389,7 +1372,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium2">
-    <tableStyle name="Estilo de Tabela Personalizado" pivot="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Estilo de Tabela Personalizado" pivot="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="33"/>
       <tableStyleElement type="headerRow" dxfId="32"/>
     </tableStyle>
@@ -1403,6 +1386,182 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="215436288"/>
+        <c:axId val="173047104"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="215436288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="173047104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="173047104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="215436288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="215750144"/>
+        <c:axId val="215172224"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="215750144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="215172224"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="215172224"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="215750144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1426,7 +1585,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26EAD538-8E63-4347-BB47-D7F21E232BE1}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26EAD538-8E63-4347-BB47-D7F21E232BE1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1502,7 +1661,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D966EEA7-9C97-45B5-8005-38D432AC4427}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D966EEA7-9C97-45B5-8005-38D432AC4427}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1578,7 +1737,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB0E7FC-D630-496A-948E-A83363D13A9B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB0E7FC-D630-496A-948E-A83363D13A9B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1654,7 +1813,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{492D2DE9-C9F9-419B-A5CF-852725D9BD6C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{492D2DE9-C9F9-419B-A5CF-852725D9BD6C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1728,6 +1887,60 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9640455" cy="6010852"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9640455" cy="6010852"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>14</xdr:col>
@@ -1747,7 +1960,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F42AA0B-FB74-4073-9E7A-B53A2A762079}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F42AA0B-FB74-4073-9E7A-B53A2A762079}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1823,7 +2036,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FDD6EB3-CB1A-478F-B360-E0A6CD273D94}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2FDD6EB3-CB1A-478F-B360-E0A6CD273D94}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1883,7 +2096,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1904,7 +2117,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ABA5CBC-9545-44BC-933C-CFDFA9B3B3CC}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9ABA5CBC-9545-44BC-933C-CFDFA9B3B3CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1964,7 +2177,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1985,7 +2198,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F90576-8ABF-49E5-9913-F219897CC146}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2F90576-8ABF-49E5-9913-F219897CC146}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2046,61 +2259,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Controlador_de_projeto" displayName="Controlador_de_projeto" ref="B4:O13" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30" tableBorderDxfId="29">
-  <autoFilter ref="B4:O13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Controlador_de_projeto" displayName="Controlador_de_projeto" ref="B4:O13" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27">
+  <autoFilter ref="B4:O13"/>
   <sortState ref="B5:O13">
     <sortCondition sortBy="icon" ref="C5:C13"/>
   </sortState>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Atividades" dataDxfId="28" dataCellStyle="Texto"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prioridade" dataDxfId="27" dataCellStyle="Texto"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Atribuída a" dataDxfId="26" dataCellStyle="Texto"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Estimado_x000a_Início" dataDxfId="25" dataCellStyle="Data"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Estimado _x000a_Término" dataDxfId="24" dataCellStyle="Data"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Trabalho Estimado (em horas)" dataDxfId="23" dataCellStyle="Números"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Duração Estimada (em dias)" dataDxfId="22" dataCellStyle="Duração estimada">
-      <calculatedColumnFormula>IF(COUNTA(Cronograma!$E5,Cronograma!$F5)&lt;&gt;2,"",DAYS360(Cronograma!$E5,Cronograma!$F5,FALSE))</calculatedColumnFormula>
+    <tableColumn id="1" name="Atividades" dataDxfId="26" dataCellStyle="Texto"/>
+    <tableColumn id="2" name="Prioridade" dataDxfId="25" dataCellStyle="Texto"/>
+    <tableColumn id="3" name="Atribuída a" dataDxfId="24" dataCellStyle="Texto"/>
+    <tableColumn id="4" name="Estimado_x000a_Início" dataDxfId="23" dataCellStyle="Data"/>
+    <tableColumn id="5" name="Estimado _x000a_Término" dataDxfId="22" dataCellStyle="Data"/>
+    <tableColumn id="6" name="Trabalho Estimado (em horas)" dataDxfId="21" dataCellStyle="Números"/>
+    <tableColumn id="7" name="Duração Estimada (em dias)" dataDxfId="20" dataCellStyle="Duração estimada">
+      <calculatedColumnFormula>E5+F5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Real _x000a_Início" dataDxfId="21" dataCellStyle="Início Real"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Real_x000a_Término" dataDxfId="20" dataCellStyle="Data"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Ícone de sinalizador para o trabalho real de acima/abaixo (em horas)" dataDxfId="19" dataCellStyle="Sinalizador">
+    <tableColumn id="8" name="Real _x000a_Início" dataDxfId="19" dataCellStyle="Início Real"/>
+    <tableColumn id="9" name="Real_x000a_Término" dataDxfId="18" dataCellStyle="Data"/>
+    <tableColumn id="10" name="Ícone de sinalizador para o trabalho real de acima/abaixo (em horas)" dataDxfId="17" dataCellStyle="Sinalizador">
       <calculatedColumnFormula>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Trabalho Real (em horas)" dataDxfId="18" dataCellStyle="Números"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Ícone de sinalizador para duração real acima/abaixo (em dias)" dataDxfId="17" dataCellStyle="Sinalizador">
+    <tableColumn id="11" name="Trabalho Real (em horas)" dataDxfId="16" dataCellStyle="Números"/>
+    <tableColumn id="12" name="Ícone de sinalizador para duração real acima/abaixo (em dias)" dataDxfId="15" dataCellStyle="Sinalizador">
       <calculatedColumnFormula>IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Duração Real (em dias)" dataDxfId="16" dataCellStyle="Coluna cinza">
+    <tableColumn id="13" name="Duração Real (em dias)" dataDxfId="14" dataCellStyle="Coluna cinza">
       <calculatedColumnFormula>IF(COUNTA(Cronograma!$I5,Cronograma!$J5)&lt;&gt;2,"",DAYS360(Cronograma!$I5,Cronograma!$J5,FALSE))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Anotações" dataDxfId="15" dataCellStyle="Texto"/>
+    <tableColumn id="14" name="Anotações" dataDxfId="13" dataCellStyle="Texto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5EF5E39F-083C-4CBF-9C73-059A3E5DC12C}" name="TabelaInformações" displayName="TabelaInformações" ref="B2:E10" totalsRowCount="1" headerRowDxfId="14" totalsRowDxfId="11" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="10">
-  <autoFilter ref="B2:E9" xr:uid="{80914F49-B214-4A9D-9AA6-C62850A3AF1D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="TabelaInformações" displayName="TabelaInformações" ref="B2:E10" totalsRowCount="1" headerRowDxfId="12" totalsRowDxfId="9" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="8">
+  <autoFilter ref="B2:E9"/>
   <sortState ref="B3:E8">
     <sortCondition ref="B2:B9"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{015C0AFA-387D-445F-B28F-76D6562120F5}" name="Nome" totalsRowFunction="count" dataDxfId="9" totalsRowDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{99352CCE-884C-490C-9AA3-B8279BA0B565}" name="E-mail" totalsRowFunction="count" dataDxfId="8" totalsRowDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{942D1AB5-65C0-4A7C-8B7B-DD05F2AB2033}" name="Celular" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{9BE67810-E51A-4696-888C-21CED24CD269}" name="Git-Hub" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="0"/>
+    <tableColumn id="1" name="Nome" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="3"/>
+    <tableColumn id="2" name="E-mail" totalsRowFunction="count" dataDxfId="6" totalsRowDxfId="2"/>
+    <tableColumn id="3" name="Celular" totalsRowFunction="count" dataDxfId="5" totalsRowDxfId="1"/>
+    <tableColumn id="4" name="Git-Hub" totalsRowFunction="count" dataDxfId="4" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="CategoryAndEmployeeTable" displayName="CategoryAndEmployeeTable" ref="B4:C17" totalsRowShown="0" headerRowCellStyle="Título 2" dataCellStyle="Texto">
-  <autoFilter ref="B4:C17" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="CategoryAndEmployeeTable" displayName="CategoryAndEmployeeTable" ref="B4:C17" totalsRowShown="0" headerRowCellStyle="Título 2" dataCellStyle="Texto">
+  <autoFilter ref="B4:C17"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Nome da Categoria" dataCellStyle="Texto"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Nome do Funcionário" dataCellStyle="Texto"/>
+    <tableColumn id="1" name="Nome da Categoria" dataCellStyle="Texto"/>
+    <tableColumn id="2" name="Nome do Funcionário" dataCellStyle="Texto"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -2337,7 +2550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB931138-51B5-4EDA-88BE-90646F168B60}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -2354,16 +2567,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1">
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2375,13 +2588,13 @@
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.875" style="1" customWidth="1"/>
     <col min="7" max="7" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.125" customWidth="1"/>
-    <col min="9" max="9" width="15.375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="2.875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12.875" customWidth="1"/>
-    <col min="13" max="13" width="2.875" customWidth="1"/>
-    <col min="14" max="14" width="13.25" customWidth="1"/>
+    <col min="8" max="8" width="13.875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.375" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="15.125" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="2.875" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.875" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="2.875" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="13.25" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="25.625" customWidth="1"/>
     <col min="16" max="16" width="2.625" customWidth="1"/>
   </cols>
@@ -2397,7 +2610,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="16.5" x14ac:dyDescent="0.3"/>
@@ -2453,45 +2666,46 @@
         <v>27</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E5" s="24">
-        <f ca="1">TODAY()+6</f>
-        <v>43545</v>
-      </c>
-      <c r="F5" s="24">
-        <f ca="1">TODAY()+30</f>
-        <v>43569</v>
+        <f>DATE(2018, 10, 1)+ 50</f>
+        <v>43424</v>
+      </c>
+      <c r="F5" s="31">
+        <f>E5+190</f>
+        <v>43614</v>
       </c>
       <c r="G5" s="25">
-        <v>210</v>
+        <f>((E5+F5)*24/360)</f>
+        <v>5802.5333333333338</v>
       </c>
       <c r="H5" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E5,Cronograma!$F5)&lt;&gt;2,"",DAYS360(Cronograma!$E5,Cronograma!$F5,FALSE))</f>
-        <v>23</v>
+        <f t="shared" ref="H5:H13" si="0">E5+F5</f>
+        <v>87038</v>
       </c>
       <c r="I5" s="27">
         <f ca="1">TODAY()-65</f>
-        <v>43474</v>
+        <v>43554</v>
       </c>
       <c r="J5" s="24">
         <f ca="1">TODAY()</f>
-        <v>43539</v>
+        <v>43619</v>
       </c>
       <c r="K5" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5" s="25">
         <v>300</v>
       </c>
       <c r="M5" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I5,Cronograma!$J5)&lt;&gt;2,"",DAYS360(Cronograma!$I5,Cronograma!$J5,FALSE))</f>
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O5" s="23"/>
     </row>
@@ -2503,30 +2717,31 @@
         <v>27</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E6" s="24">
-        <f ca="1">TODAY()-35</f>
-        <v>43504</v>
+        <f>DATE(2018, 10, 1)</f>
+        <v>43374</v>
       </c>
       <c r="F6" s="24">
-        <f ca="1">TODAY()+20</f>
-        <v>43559</v>
+        <f>E6+250</f>
+        <v>43624</v>
       </c>
       <c r="G6" s="25">
-        <v>400</v>
+        <f>((E6+F6)*24/360)</f>
+        <v>5799.8666666666668</v>
       </c>
       <c r="H6" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E6,Cronograma!$F6)&lt;&gt;2,"",DAYS360(Cronograma!$E6,Cronograma!$F6,FALSE))</f>
-        <v>56</v>
+        <f t="shared" si="0"/>
+        <v>86998</v>
       </c>
       <c r="I6" s="27">
         <f ca="1">TODAY()-41</f>
-        <v>43498</v>
+        <v>43578</v>
       </c>
       <c r="J6" s="24">
         <f ca="1">TODAY()-7</f>
-        <v>43532</v>
+        <v>43612</v>
       </c>
       <c r="K6" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
@@ -2537,11 +2752,11 @@
       </c>
       <c r="M6" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I6,Cronograma!$J6)&lt;&gt;2,"",DAYS360(Cronograma!$I6,Cronograma!$J6,FALSE))</f>
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O6" s="23" t="s">
         <v>40</v>
@@ -2558,27 +2773,28 @@
         <v>33</v>
       </c>
       <c r="E7" s="24">
-        <f ca="1">TODAY()+8</f>
-        <v>43547</v>
+        <f>DATE(2019, 3, 18)</f>
+        <v>43542</v>
       </c>
       <c r="F7" s="24">
-        <f ca="1">TODAY()+30</f>
-        <v>43569</v>
+        <f>E7+1</f>
+        <v>43543</v>
       </c>
       <c r="G7" s="25">
-        <v>500</v>
+        <f>((E7+F7)*24/360)</f>
+        <v>5805.666666666667</v>
       </c>
       <c r="H7" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E7,Cronograma!$F7)&lt;&gt;2,"",DAYS360(Cronograma!$E7,Cronograma!$F7,FALSE))</f>
-        <v>21</v>
+        <f t="shared" si="0"/>
+        <v>87085</v>
       </c>
       <c r="I7" s="27">
         <f ca="1">TODAY()-100</f>
-        <v>43439</v>
+        <v>43519</v>
       </c>
       <c r="J7" s="24">
         <f ca="1">TODAY()-27</f>
-        <v>43512</v>
+        <v>43592</v>
       </c>
       <c r="K7" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
@@ -2589,11 +2805,11 @@
       </c>
       <c r="M7" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I7,Cronograma!$J7)&lt;&gt;2,"",DAYS360(Cronograma!$I7,Cronograma!$J7,FALSE))</f>
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="O7" s="23"/>
     </row>
@@ -2608,27 +2824,27 @@
         <v>33</v>
       </c>
       <c r="E8" s="24">
-        <f ca="1">TODAY()+9</f>
-        <v>43548</v>
+        <f>DATE(2019, 3, 18)</f>
+        <v>43542</v>
       </c>
       <c r="F8" s="24">
-        <f ca="1">TODAY()+30</f>
-        <v>43569</v>
+        <f>F7</f>
+        <v>43543</v>
       </c>
       <c r="G8" s="25">
         <v>250</v>
       </c>
       <c r="H8" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E8,Cronograma!$F8)&lt;&gt;2,"",DAYS360(Cronograma!$E8,Cronograma!$F8,FALSE))</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>87085</v>
       </c>
       <c r="I8" s="27">
         <f ca="1">TODAY()-90</f>
-        <v>43449</v>
+        <v>43529</v>
       </c>
       <c r="J8" s="24">
         <f ca="1">TODAY()-71</f>
-        <v>43468</v>
+        <v>43548</v>
       </c>
       <c r="K8" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
@@ -2643,7 +2859,7 @@
       </c>
       <c r="N8" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I8,Cronograma!$J8)&lt;&gt;2,"",DAYS360(Cronograma!$I8,Cronograma!$J8,FALSE))</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O8" s="23"/>
     </row>
@@ -2655,30 +2871,31 @@
         <v>26</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E9" s="24">
-        <f ca="1">TODAY()+10</f>
-        <v>43549</v>
+        <f>DATE(2019,4,2)</f>
+        <v>43557</v>
       </c>
       <c r="F9" s="24">
-        <f ca="1">TODAY()+30</f>
-        <v>43569</v>
+        <f>E9+65</f>
+        <v>43622</v>
       </c>
       <c r="G9" s="25">
-        <v>300</v>
+        <f>((E9+F9)*24/360)</f>
+        <v>5811.9333333333334</v>
       </c>
       <c r="H9" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E9,Cronograma!$F9)&lt;&gt;2,"",DAYS360(Cronograma!$E9,Cronograma!$F9,FALSE))</f>
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>87179</v>
       </c>
       <c r="I9" s="27">
         <f ca="1">TODAY()-90</f>
-        <v>43449</v>
+        <v>43529</v>
       </c>
       <c r="J9" s="24">
         <f ca="1">TODAY()-44</f>
-        <v>43495</v>
+        <v>43575</v>
       </c>
       <c r="K9" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
@@ -2689,7 +2906,7 @@
       </c>
       <c r="M9" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I9,Cronograma!$J9)&lt;&gt;2,"",DAYS360(Cronograma!$I9,Cronograma!$J9,FALSE))</f>
@@ -2708,31 +2925,31 @@
         <v>33</v>
       </c>
       <c r="E10" s="24">
-        <f ca="1">TODAY()+11</f>
-        <v>43550</v>
+        <f>DATE(2019,5,9)</f>
+        <v>43594</v>
       </c>
       <c r="F10" s="24">
-        <f ca="1">TODAY()+30</f>
-        <v>43569</v>
+        <f>E10+1</f>
+        <v>43595</v>
       </c>
       <c r="G10" s="25">
-        <v>500</v>
+        <v>24</v>
       </c>
       <c r="H10" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E10,Cronograma!$F10)&lt;&gt;2,"",DAYS360(Cronograma!$E10,Cronograma!$F10,FALSE))</f>
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>87189</v>
       </c>
       <c r="I10" s="27">
         <f ca="1">TODAY()-60</f>
-        <v>43479</v>
+        <v>43559</v>
       </c>
       <c r="J10" s="24">
         <f ca="1">TODAY()-45</f>
-        <v>43494</v>
+        <v>43574</v>
       </c>
       <c r="K10" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L10" s="25">
         <v>510</v>
@@ -2758,42 +2975,43 @@
         <v>35</v>
       </c>
       <c r="E11" s="24">
-        <f ca="1">TODAY()-44</f>
-        <v>43495</v>
+        <f>DATE(2019,5,14)</f>
+        <v>43599</v>
       </c>
       <c r="F11" s="24">
-        <f ca="1">TODAY()+30</f>
-        <v>43569</v>
+        <f>E11+1</f>
+        <v>43600</v>
       </c>
       <c r="G11" s="25">
-        <v>750</v>
+        <f>G10</f>
+        <v>24</v>
       </c>
       <c r="H11" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E11,Cronograma!$F11)&lt;&gt;2,"",DAYS360(Cronograma!$E11,Cronograma!$F11,FALSE))</f>
-        <v>74</v>
+        <f t="shared" si="0"/>
+        <v>87199</v>
       </c>
       <c r="I11" s="27">
         <f ca="1">TODAY()-44</f>
-        <v>43495</v>
+        <v>43575</v>
       </c>
       <c r="J11" s="24">
         <f ca="1">TODAY()-15</f>
-        <v>43524</v>
+        <v>43604</v>
       </c>
       <c r="K11" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L11" s="25">
         <v>790</v>
       </c>
       <c r="M11" s="28">
         <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I11,Cronograma!$J11)&lt;&gt;2,"",DAYS360(Cronograma!$I11,Cronograma!$J11,FALSE))</f>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O11" s="23"/>
     </row>
@@ -2808,27 +3026,28 @@
         <v>38</v>
       </c>
       <c r="E12" s="24">
-        <f ca="1">TODAY()+20</f>
-        <v>43559</v>
+        <f>DATE(2019, 5, 20)</f>
+        <v>43605</v>
       </c>
       <c r="F12" s="24">
-        <f ca="1">TODAY()+60</f>
-        <v>43599</v>
+        <f>E12+20</f>
+        <v>43625</v>
       </c>
       <c r="G12" s="25">
-        <v>450</v>
+        <f>15*24</f>
+        <v>360</v>
       </c>
       <c r="H12" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E12,Cronograma!$F12)&lt;&gt;2,"",DAYS360(Cronograma!$E12,Cronograma!$F12,FALSE))</f>
-        <v>40</v>
+        <f t="shared" si="0"/>
+        <v>87230</v>
       </c>
       <c r="I12" s="27">
         <f ca="1">TODAY()-45</f>
-        <v>43494</v>
+        <v>43574</v>
       </c>
       <c r="J12" s="24">
         <f ca="1">TODAY()-5</f>
-        <v>43534</v>
+        <v>43614</v>
       </c>
       <c r="K12" s="28">
         <f>IFERROR(IF(Controlador_de_projeto[Trabalho Real (em horas)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Trabalho Real (em horas)]]-Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])/Controlador_de_projeto[[#This Row],[Trabalho Estimado (em horas)]])&gt;FlagPercent,1,0)),"")</f>
@@ -2843,7 +3062,7 @@
       </c>
       <c r="N12" s="29">
         <f ca="1">IF(COUNTA(Cronograma!$I12,Cronograma!$J12)&lt;&gt;2,"",DAYS360(Cronograma!$I12,Cronograma!$J12,FALSE))</f>
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O12" s="23"/>
     </row>
@@ -2855,22 +3074,23 @@
         <v>26</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E13" s="24">
-        <f ca="1">TODAY()-160</f>
-        <v>43379</v>
+        <f>DATE(2018, 11, 2)</f>
+        <v>43406</v>
       </c>
       <c r="F13" s="24">
-        <f ca="1">TODAY()+91</f>
-        <v>43630</v>
+        <f>E13+215</f>
+        <v>43621</v>
       </c>
       <c r="G13" s="25">
-        <v>250</v>
+        <f>(E13+F13)*24/360</f>
+        <v>5801.8</v>
       </c>
       <c r="H13" s="26">
-        <f ca="1">IF(COUNTA(Cronograma!$E13,Cronograma!$F13)&lt;&gt;2,"",DAYS360(Cronograma!$E13,Cronograma!$F13,FALSE))</f>
-        <v>248</v>
+        <f t="shared" si="0"/>
+        <v>87027</v>
       </c>
       <c r="I13" s="27">
         <v>42434</v>
@@ -2886,8 +3106,8 @@
         <v>200</v>
       </c>
       <c r="M13" s="28">
-        <f ca="1">IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
-        <v>1</v>
+        <f>IFERROR(IF(Controlador_de_projeto[Duração Real (em dias)]=0,"",IF(ABS((Controlador_de_projeto[[#This Row],[Duração Real (em dias)]]-Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])/Controlador_de_projeto[[#This Row],[Duração Estimada (em dias)]])&gt;FlagPercent,1,0)),"")</f>
+        <v>0</v>
       </c>
       <c r="N13" s="29">
         <f>IF(COUNTA(Cronograma!$I13,Cronograma!$J13)&lt;&gt;2,"",DAYS360(Cronograma!$I13,Cronograma!$J13,FALSE))</f>
@@ -2900,38 +3120,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L5:L13">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="31" priority="6">
       <formula>(ABS((L5-G5))/G5)&gt;FlagPercent</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:N13">
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>(ABS((N5-H5))/H5)&gt;FlagPercent</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="18">
-    <dataValidation allowBlank="1" showInputMessage="1" prompt="Insira projetos nesta planilha de controle. Defina a porcentagem a sinalizar em D2. Trabalho real em horas e duração real em dias destacará valores acima/abaixo com o estilo de fonte em negrito vermelho e um ícone de sinalizador nas colunas K e M " sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Porcentagem acima/abaixo personalizáveis usadas para realçar o trabalho real em horas e dias na tabela de projetos que excedam ou fiquem abaixo deste número" sqref="C2" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="C5:C13" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="Insira projetos nesta planilha de controle. Defina a porcentagem a sinalizar em D2. Trabalho real em horas e duração real em dias destacará valores acima/abaixo com o estilo de fonte em negrito vermelho e um ícone de sinalizador nas colunas K e M " sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Porcentagem acima/abaixo personalizáveis usadas para realçar o trabalho real em horas e dias na tabela de projetos que excedam ou fiquem abaixo deste número" sqref="C2"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione uma categoria na lista ou crie uma nova categoria para exibir nesta lista da planilha Configuração." sqref="C5:C13">
       <formula1>CategoryList</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione um funcionário na lista ou crie um novo funcionário para exibir nesta lista da planilha Configuração." sqref="D5:D13" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Selecione um funcionário na lista ou crie um novo funcionário para exibir nesta lista da planilha Configuração." sqref="D5:D13">
       <formula1>EmployeeList</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira nomes de projetos desta coluna" sqref="B4" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione um nome de Categoria na lista suspensa em cada célula nesta coluna. As opções nesta lista são definidas na planilha Configuração. Pressione Alt+Seta para baixo para navegar pela lista e Enter para fazer uma seleção" sqref="C4" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione o nome do Funcionário na lista suspensa em cada célula nesta coluna. As opções são definidas na planilha Configuração. Pressione Alt+Seta para baixo para navegar pela lista e Enter para fazer uma seleção" sqref="D4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de início estimada do projeto nesta coluna" sqref="E4" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de término estimada do projeto nesta coluna" sqref="F4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira o trabalho estimado do projeto em horas" sqref="G4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a duração estimada do projeto em dias nesta coluna" sqref="H4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de início real do projeto nesta coluna" sqref="I4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de término real do projeto nesta coluna" sqref="J4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sinalizador do título da tabela Controlador de projeto em Trabalho Real Acima/Abaixo (em horas). Valores na coluna L que atendem aos critérios geram sinalizadores nas células da coluna. Células em branco indicam valores que não atendem aos critérios" sqref="K4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sinalizador do título da tabela Controlador de projeto da Duração Acima/Abaixo (em dias). Valores na coluna N que atendem aos critérios geram sinalizadores nas células desta coluna. Células em branco indicam valores que não atendem aos critérios" sqref="M4" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira o trabalho do real do projeto em horas. Valores que atendem aos critérios Acima/Abaixo são destacados em negrito vermelho e geram um ícone de sinalizador na coluna K à esquerda" sqref="L4" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a duração real do projeto em dias. Os valores que atendem aos critérios Acima/Abaixo são destacados em vermelho negrito e geram um ícone sinalizador na coluna M à esquerda" sqref="N4" xr:uid="{00000000-0002-0000-0000-000010000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira anotações para os projetos nesta coluna" sqref="O4" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira nomes de projetos desta coluna" sqref="B4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione um nome de Categoria na lista suspensa em cada célula nesta coluna. As opções nesta lista são definidas na planilha Configuração. Pressione Alt+Seta para baixo para navegar pela lista e Enter para fazer uma seleção" sqref="C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Selecione o nome do Funcionário na lista suspensa em cada célula nesta coluna. As opções são definidas na planilha Configuração. Pressione Alt+Seta para baixo para navegar pela lista e Enter para fazer uma seleção" sqref="D4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de início estimada do projeto nesta coluna" sqref="E4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de término estimada do projeto nesta coluna" sqref="F4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira o trabalho estimado do projeto em horas" sqref="G4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a duração estimada do projeto em dias nesta coluna" sqref="H4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de início real do projeto nesta coluna" sqref="I4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a data de término real do projeto nesta coluna" sqref="J4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sinalizador do título da tabela Controlador de projeto em Trabalho Real Acima/Abaixo (em horas). Valores na coluna L que atendem aos critérios geram sinalizadores nas células da coluna. Células em branco indicam valores que não atendem aos critérios" sqref="K4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Sinalizador do título da tabela Controlador de projeto da Duração Acima/Abaixo (em dias). Valores na coluna N que atendem aos critérios geram sinalizadores nas células desta coluna. Células em branco indicam valores que não atendem aos critérios" sqref="M4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira o trabalho do real do projeto em horas. Valores que atendem aos critérios Acima/Abaixo são destacados em negrito vermelho e geram um ícone de sinalizador na coluna K à esquerda" sqref="L4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira a duração real do projeto em dias. Os valores que atendem aos critérios Acima/Abaixo são destacados em vermelho negrito e geram um ícone sinalizador na coluna M à esquerda" sqref="N4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira anotações para os projetos nesta coluna" sqref="O4"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
@@ -2991,11 +3211,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DD9322-CF5B-4EA7-B626-99B03376E7BD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3128,15 +3348,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{10E1A243-1F9D-4653-9CB3-246FAAEFFFC9}"/>
-    <hyperlink ref="C4" r:id="rId2" xr:uid="{5E2A8B4C-3175-420D-9022-5F5D373DE07E}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{A208A63A-DA4E-48D4-ACA4-51055CB62F93}"/>
-    <hyperlink ref="E3" r:id="rId4" xr:uid="{6E583752-D9C6-4B44-A385-99315902FAAA}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{8169B9CF-DAC7-4769-B26B-3A29711DE9E2}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{9ACC969C-4C4F-4DD2-9241-A3B590E23052}"/>
-    <hyperlink ref="E9" r:id="rId7" xr:uid="{4AFB3E2B-1BA3-4670-9BC2-50B1056D2DED}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{613390DA-BE61-41F9-8193-624ACF60D985}"/>
-    <hyperlink ref="C5" r:id="rId9" xr:uid="{B644CA9E-9055-46BC-9292-573A237280C1}"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId4"/>
+    <hyperlink ref="E5" r:id="rId5"/>
+    <hyperlink ref="E7" r:id="rId6"/>
+    <hyperlink ref="E9" r:id="rId7"/>
+    <hyperlink ref="E8" r:id="rId8"/>
+    <hyperlink ref="C5" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId10"/>
@@ -3147,7 +3367,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2">
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
@@ -3167,10 +3387,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="31"/>
+      <c r="C1" s="32"/>
     </row>
     <row r="2" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3265,9 +3485,9 @@
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation allowBlank="1" showInputMessage="1" prompt="A planilha de configuração contém uma lista personalizável de categorias de projeto e nomes dos funcionários. Essas listas são usadas como listas suspensas na planilha de controle de projetos. As listas não precisam do mesmo número de itens entre elas " sqref="A1" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira os nomes de funcionários nesta coluna que serão usados como opções na lista suspensa Atribuído a na planilha Controlador de projeto" sqref="C4" xr:uid="{00000000-0002-0000-0100-000001000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira as categorias de projeto nesta coluna que serão usadas como opções na lista suspensa Categoria na planilha Controlador de projeto" sqref="B4" xr:uid="{00000000-0002-0000-0100-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" prompt="A planilha de configuração contém uma lista personalizável de categorias de projeto e nomes dos funcionários. Essas listas são usadas como listas suspensas na planilha de controle de projetos. As listas não precisam do mesmo número de itens entre elas " sqref="A1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira os nomes de funcionários nesta coluna que serão usados como opções na lista suspensa Atribuído a na planilha Controlador de projeto" sqref="C4"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Insira as categorias de projeto nesta coluna que serão usadas como opções na lista suspensa Categoria na planilha Controlador de projeto" sqref="B4"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>